<commit_message>
Added high current 3.3v supply
</commit_message>
<xml_diff>
--- a/CM4/DataSheets/KeyboardMatrixMap.xlsx
+++ b/CM4/DataSheets/KeyboardMatrixMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hailey\Desktop\Current ti92Project\TI92-revive-main\TI92-RPI-Zero\CM4\DataSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE2758F4-FF24-471D-8E68-787C711AC0C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49EA5BBA-D214-43E7-B940-E6787AB59C38}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14940" yWindow="3150" windowWidth="18000" windowHeight="9360" xr2:uid="{8BC75FC5-BF04-4A58-94D3-06EA8DB1ADCD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{8BC75FC5-BF04-4A58-94D3-06EA8DB1ADCD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -624,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B4FF08F-8B4A-49EC-9E50-CA9C945A3C1B}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>